<commit_message>
✨ Refactor comparador and parser_invoice for improved validation and error handling; update column normalization and checks in confrontar function.
</commit_message>
<xml_diff>
--- a/utils/modelo_invoice.xlsx
+++ b/utils/modelo_invoice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodolfo\Documents\codigos\git\confronto_nfe_invoice\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodolfo\Desktop\confronto_nfe_invoice\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEB7501-F0E2-4A36-81BD-56D0969B227C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC82A80-3A6B-492F-A254-7B87FC148AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>marca</t>
   </si>
@@ -47,62 +47,33 @@
     <t>cor</t>
   </si>
   <si>
-    <t>bra_dummy</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>cajas</t>
-  </si>
-  <si>
     <t>total pares</t>
   </si>
   <si>
-    <t>unit price</t>
-  </si>
-  <si>
     <t>valor total</t>
   </si>
   <si>
     <t>item</t>
+  </si>
+  <si>
+    <t>caixas</t>
+  </si>
+  <si>
+    <t>preco unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,14 +99,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 12" xfId="1" xr:uid="{2F0C27A8-8867-40B3-BCAB-50222164E132}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,17 +408,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="AM20" sqref="AM20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="31" width="5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -459,53 +435,95 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1">
+        <v>20</v>
+      </c>
+      <c r="G1">
+        <v>21</v>
+      </c>
+      <c r="H1">
+        <v>22</v>
+      </c>
+      <c r="I1">
+        <v>23</v>
+      </c>
+      <c r="J1">
+        <v>24</v>
+      </c>
+      <c r="K1">
+        <v>25</v>
+      </c>
+      <c r="L1">
+        <v>26</v>
+      </c>
+      <c r="M1">
+        <v>27</v>
+      </c>
+      <c r="N1">
+        <v>28</v>
+      </c>
+      <c r="O1">
+        <v>29</v>
+      </c>
+      <c r="P1">
+        <v>30</v>
+      </c>
+      <c r="Q1">
+        <v>31</v>
+      </c>
+      <c r="R1">
+        <v>32</v>
+      </c>
+      <c r="S1">
+        <v>33</v>
+      </c>
+      <c r="T1">
+        <v>34</v>
+      </c>
+      <c r="U1">
+        <v>35</v>
+      </c>
+      <c r="V1">
+        <v>36</v>
+      </c>
+      <c r="W1">
+        <v>37</v>
+      </c>
+      <c r="X1">
+        <v>38</v>
+      </c>
+      <c r="Y1">
+        <v>39</v>
+      </c>
+      <c r="Z1">
+        <v>40</v>
+      </c>
+      <c r="AA1">
+        <v>41</v>
+      </c>
+      <c r="AB1">
+        <v>42</v>
+      </c>
+      <c r="AC1">
+        <v>43</v>
+      </c>
+      <c r="AD1">
+        <v>44</v>
+      </c>
+      <c r="AE1">
+        <v>45</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="AH1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>